<commit_message>
gate driver, voltage sense board and regulation
</commit_message>
<xml_diff>
--- a/doc/calculations.xlsx
+++ b/doc/calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UwesTechnik\stepup-test\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199E7E00-5197-47B8-98F6-FFB34C7C31C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A21D643-089E-441D-B65D-07BB17B3B54E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1635" yWindow="300" windowWidth="18375" windowHeight="10470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
   <si>
     <t>U_in [V]</t>
   </si>
@@ -75,6 +75,24 @@
   </si>
   <si>
     <t>3. D + (100nF || 12k) spike-smoothing</t>
+  </si>
+  <si>
+    <t>With "Level 6: The gate driver"</t>
+  </si>
+  <si>
+    <t>7 gates of 74HC08 in parallel, to drive the FET.</t>
+  </si>
+  <si>
+    <t>Before</t>
+  </si>
+  <si>
+    <t>After</t>
+  </si>
+  <si>
+    <t>Conclusion: The edges are sharper by ~factor 2. The efficiency stays the same. There is nearly no heating of the FET.</t>
+  </si>
+  <si>
+    <t>With "Level 7: Voltage regulation"</t>
   </si>
 </sst>
 </file>
@@ -175,6 +193,138 @@
         <a:xfrm>
           <a:off x="6115202" y="85725"/>
           <a:ext cx="5001804" cy="3753849"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>441317</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>44822</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>72510</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BD82CE8-776B-1AD4-E8FE-0B98205138A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5988229" y="4616822"/>
+          <a:ext cx="4466859" cy="3075688"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>174812</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>67236</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>246178</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>101784</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Grafik 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5344B52-9A90-9965-9DCD-8253113EA4E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1385047" y="4639236"/>
+          <a:ext cx="4408043" cy="3082548"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47452</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>78439</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>589651</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>137158</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Grafik 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{495F02DB-A611-17BF-3226-C12B70190262}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1257687" y="11127439"/>
+          <a:ext cx="7176082" cy="5392719"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -449,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:J16"/>
+  <dimension ref="B2:K99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N94" sqref="N94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,27 +689,27 @@
         <v>2</v>
       </c>
       <c r="E8">
-        <f>E6*E7</f>
+        <f t="shared" ref="E8:J8" si="0">E6*E7</f>
         <v>8.82</v>
       </c>
       <c r="F8">
-        <f>F6*F7</f>
+        <f t="shared" si="0"/>
         <v>7.7279999999999989</v>
       </c>
       <c r="G8">
-        <f>G6*G7</f>
+        <f t="shared" si="0"/>
         <v>6.375</v>
       </c>
       <c r="H8">
-        <f>H6*H7</f>
+        <f t="shared" si="0"/>
         <v>4.95</v>
       </c>
       <c r="I8">
-        <f>I6*I7</f>
+        <f t="shared" si="0"/>
         <v>3.88</v>
       </c>
       <c r="J8">
-        <f>J6*J7</f>
+        <f t="shared" si="0"/>
         <v>2.2199999999999998</v>
       </c>
     </row>
@@ -615,27 +765,27 @@
         <v>5</v>
       </c>
       <c r="E12">
-        <f>E10/E11</f>
+        <f t="shared" ref="E12:J12" si="1">E10/E11</f>
         <v>6.65</v>
       </c>
       <c r="F12">
-        <f>F10/F11</f>
+        <f t="shared" si="1"/>
         <v>6.41</v>
       </c>
       <c r="G12">
-        <f>G10/G11</f>
+        <f t="shared" si="1"/>
         <v>5.88</v>
       </c>
       <c r="H12">
-        <f>H10/H11</f>
+        <f t="shared" si="1"/>
         <v>5.25</v>
       </c>
       <c r="I12">
-        <f>I10/I11</f>
+        <f t="shared" si="1"/>
         <v>4.6900000000000004</v>
       </c>
       <c r="J12">
-        <f>J10/J11</f>
+        <f t="shared" si="1"/>
         <v>3.59</v>
       </c>
     </row>
@@ -644,27 +794,27 @@
         <v>6</v>
       </c>
       <c r="E13" s="1">
-        <f>E10*E12/1000</f>
+        <f t="shared" ref="E13:J13" si="2">E10*E12/1000</f>
         <v>4.42225</v>
       </c>
       <c r="F13" s="1">
-        <f>F10*F12/1000</f>
+        <f t="shared" si="2"/>
         <v>4.1088100000000001</v>
       </c>
       <c r="G13" s="1">
-        <f>G10*G12/1000</f>
+        <f t="shared" si="2"/>
         <v>3.4574400000000001</v>
       </c>
       <c r="H13" s="1">
-        <f>H10*H12/1000</f>
+        <f t="shared" si="2"/>
         <v>2.7562500000000001</v>
       </c>
       <c r="I13" s="1">
-        <f>I10*I12/1000</f>
+        <f t="shared" si="2"/>
         <v>2.1996100000000003</v>
       </c>
       <c r="J13" s="1">
-        <f>J10*J12/1000</f>
+        <f t="shared" si="2"/>
         <v>1.28881</v>
       </c>
     </row>
@@ -681,27 +831,27 @@
         <v>8</v>
       </c>
       <c r="E15" s="1">
-        <f>E8-E13</f>
+        <f t="shared" ref="E15:J15" si="3">E8-E13</f>
         <v>4.3977500000000003</v>
       </c>
       <c r="F15" s="1">
-        <f>F8-F13</f>
+        <f t="shared" si="3"/>
         <v>3.6191899999999988</v>
       </c>
       <c r="G15" s="1">
-        <f>G8-G13</f>
+        <f t="shared" si="3"/>
         <v>2.9175599999999999</v>
       </c>
       <c r="H15" s="1">
-        <f>H8-H13</f>
+        <f t="shared" si="3"/>
         <v>2.1937500000000001</v>
       </c>
       <c r="I15" s="1">
-        <f>I8-I13</f>
+        <f t="shared" si="3"/>
         <v>1.6803899999999996</v>
       </c>
       <c r="J15" s="1">
-        <f>J8-J13</f>
+        <f t="shared" si="3"/>
         <v>0.93118999999999974</v>
       </c>
     </row>
@@ -710,28 +860,585 @@
         <v>7</v>
       </c>
       <c r="E16" s="1">
-        <f>E13/E8</f>
+        <f t="shared" ref="E16:J16" si="4">E13/E8</f>
         <v>0.50138888888888888</v>
       </c>
       <c r="F16" s="1">
-        <f>F13/F8</f>
+        <f t="shared" si="4"/>
         <v>0.53167831262939969</v>
       </c>
       <c r="G16" s="1">
-        <f>G13/G8</f>
+        <f t="shared" si="4"/>
         <v>0.54234352941176467</v>
       </c>
       <c r="H16" s="1">
-        <f>H13/H8</f>
+        <f t="shared" si="4"/>
         <v>0.55681818181818177</v>
       </c>
       <c r="I16" s="1">
-        <f>I13/I8</f>
+        <f t="shared" si="4"/>
         <v>0.56690979381443307</v>
       </c>
       <c r="J16" s="1">
-        <f>J13/J8</f>
+        <f t="shared" si="4"/>
         <v>0.58054504504504512</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c r="K24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C44" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2">
+        <v>5.3</v>
+      </c>
+      <c r="F44" s="2">
+        <v>5</v>
+      </c>
+      <c r="G44" s="2">
+        <v>4</v>
+      </c>
+      <c r="H44" s="2">
+        <v>3</v>
+      </c>
+      <c r="I44" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="J44" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C45" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2">
+        <v>1.27</v>
+      </c>
+      <c r="F45" s="2">
+        <v>1.21</v>
+      </c>
+      <c r="G45" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="H45" s="2">
+        <v>0.74</v>
+      </c>
+      <c r="I45" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="J45" s="2">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <f t="shared" ref="E46" si="5">E44*E45</f>
+        <v>6.7309999999999999</v>
+      </c>
+      <c r="F46">
+        <f t="shared" ref="F46" si="6">F44*F45</f>
+        <v>6.05</v>
+      </c>
+      <c r="G46">
+        <f t="shared" ref="G46" si="7">G44*G45</f>
+        <v>3.88</v>
+      </c>
+      <c r="H46">
+        <f t="shared" ref="H46" si="8">H44*H45</f>
+        <v>2.2199999999999998</v>
+      </c>
+      <c r="I46">
+        <f t="shared" ref="I46" si="9">I44*I45</f>
+        <v>1.55</v>
+      </c>
+      <c r="J46">
+        <f t="shared" ref="J46" si="10">J44*J45</f>
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C48" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2">
+        <v>600</v>
+      </c>
+      <c r="F48" s="2">
+        <v>570</v>
+      </c>
+      <c r="G48" s="2">
+        <v>457</v>
+      </c>
+      <c r="H48" s="2">
+        <v>347</v>
+      </c>
+      <c r="I48" s="2">
+        <v>290</v>
+      </c>
+      <c r="J48" s="2">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>4</v>
+      </c>
+      <c r="E49">
+        <v>100</v>
+      </c>
+      <c r="F49">
+        <v>100</v>
+      </c>
+      <c r="G49">
+        <v>100</v>
+      </c>
+      <c r="H49">
+        <v>100</v>
+      </c>
+      <c r="I49">
+        <v>100</v>
+      </c>
+      <c r="J49">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50">
+        <f t="shared" ref="E50" si="11">E48/E49</f>
+        <v>6</v>
+      </c>
+      <c r="F50">
+        <f t="shared" ref="F50" si="12">F48/F49</f>
+        <v>5.7</v>
+      </c>
+      <c r="G50">
+        <f t="shared" ref="G50" si="13">G48/G49</f>
+        <v>4.57</v>
+      </c>
+      <c r="H50">
+        <f t="shared" ref="H50" si="14">H48/H49</f>
+        <v>3.47</v>
+      </c>
+      <c r="I50">
+        <f t="shared" ref="I50" si="15">I48/I49</f>
+        <v>2.9</v>
+      </c>
+      <c r="J50">
+        <f t="shared" ref="J50" si="16">J48/J49</f>
+        <v>2.27</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" s="1">
+        <f t="shared" ref="E51" si="17">E48*E50/1000</f>
+        <v>3.6</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" ref="F51" si="18">F48*F50/1000</f>
+        <v>3.2490000000000001</v>
+      </c>
+      <c r="G51" s="1">
+        <f t="shared" ref="G51" si="19">G48*G50/1000</f>
+        <v>2.0884900000000002</v>
+      </c>
+      <c r="H51" s="1">
+        <f t="shared" ref="H51" si="20">H48*H50/1000</f>
+        <v>1.2040900000000001</v>
+      </c>
+      <c r="I51" s="1">
+        <f t="shared" ref="I51" si="21">I48*I50/1000</f>
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="J51" s="1">
+        <f t="shared" ref="J51" si="22">J48*J50/1000</f>
+        <v>0.51528999999999991</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" ref="E53:J53" si="23">E46-E51</f>
+        <v>3.1309999999999998</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="23"/>
+        <v>2.8009999999999997</v>
+      </c>
+      <c r="G53" s="1">
+        <f t="shared" si="23"/>
+        <v>1.7915099999999997</v>
+      </c>
+      <c r="H53" s="1">
+        <f t="shared" si="23"/>
+        <v>1.0159099999999996</v>
+      </c>
+      <c r="I53" s="1">
+        <f t="shared" si="23"/>
+        <v>0.70900000000000007</v>
+      </c>
+      <c r="J53" s="1">
+        <f t="shared" si="23"/>
+        <v>0.46471000000000007</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="1">
+        <f t="shared" ref="E54:J54" si="24">E51/E46</f>
+        <v>0.53483880552666763</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="24"/>
+        <v>0.53702479338842979</v>
+      </c>
+      <c r="G54" s="1">
+        <f t="shared" si="24"/>
+        <v>0.53827061855670111</v>
+      </c>
+      <c r="H54" s="1">
+        <f t="shared" si="24"/>
+        <v>0.54238288288288294</v>
+      </c>
+      <c r="I54" s="1">
+        <f t="shared" si="24"/>
+        <v>0.54258064516129034</v>
+      </c>
+      <c r="J54" s="1">
+        <f t="shared" si="24"/>
+        <v>0.52580612244897951</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="89" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C89" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2">
+        <v>6</v>
+      </c>
+      <c r="F89" s="2">
+        <v>5</v>
+      </c>
+      <c r="G89" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="H89" s="2">
+        <v>4</v>
+      </c>
+      <c r="I89" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="J89" s="2">
+        <v>3</v>
+      </c>
+      <c r="K89" s="2">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="90" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C90" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="F90" s="2">
+        <v>0.39</v>
+      </c>
+      <c r="G90" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="H90" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I90" s="2">
+        <v>0.61</v>
+      </c>
+      <c r="J90" s="2">
+        <v>0.73</v>
+      </c>
+      <c r="K90" s="2">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="91" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
+        <v>2</v>
+      </c>
+      <c r="E91">
+        <f t="shared" ref="E91:J91" si="25">E89*E90</f>
+        <v>1.92</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="25"/>
+        <v>1.9500000000000002</v>
+      </c>
+      <c r="G91">
+        <f t="shared" si="25"/>
+        <v>2.0249999999999999</v>
+      </c>
+      <c r="H91">
+        <f t="shared" si="25"/>
+        <v>2</v>
+      </c>
+      <c r="I91">
+        <f t="shared" si="25"/>
+        <v>2.1349999999999998</v>
+      </c>
+      <c r="J91">
+        <f t="shared" si="25"/>
+        <v>2.19</v>
+      </c>
+      <c r="K91">
+        <f t="shared" ref="K91" si="26">K89*K90</f>
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="93" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C93" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2">
+        <v>350</v>
+      </c>
+      <c r="F93" s="2">
+        <v>350</v>
+      </c>
+      <c r="G93" s="2">
+        <v>350</v>
+      </c>
+      <c r="H93" s="2">
+        <v>350</v>
+      </c>
+      <c r="I93" s="2">
+        <v>350</v>
+      </c>
+      <c r="J93" s="2">
+        <v>346</v>
+      </c>
+      <c r="K93" s="2">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="94" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
+        <v>4</v>
+      </c>
+      <c r="E94">
+        <v>100</v>
+      </c>
+      <c r="F94">
+        <v>100</v>
+      </c>
+      <c r="G94">
+        <v>100</v>
+      </c>
+      <c r="H94">
+        <v>100</v>
+      </c>
+      <c r="I94">
+        <v>100</v>
+      </c>
+      <c r="J94">
+        <v>100</v>
+      </c>
+      <c r="K94">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="95" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
+        <v>5</v>
+      </c>
+      <c r="E95">
+        <f t="shared" ref="E95:J95" si="27">E93/E94</f>
+        <v>3.5</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="27"/>
+        <v>3.5</v>
+      </c>
+      <c r="G95">
+        <f t="shared" si="27"/>
+        <v>3.5</v>
+      </c>
+      <c r="H95">
+        <f t="shared" si="27"/>
+        <v>3.5</v>
+      </c>
+      <c r="I95">
+        <f t="shared" si="27"/>
+        <v>3.5</v>
+      </c>
+      <c r="J95">
+        <f t="shared" si="27"/>
+        <v>3.46</v>
+      </c>
+      <c r="K95">
+        <f t="shared" ref="K95" si="28">K93/K94</f>
+        <v>2.92</v>
+      </c>
+    </row>
+    <row r="96" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
+        <v>6</v>
+      </c>
+      <c r="E96" s="1">
+        <f t="shared" ref="E96:J96" si="29">E93*E95/1000</f>
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="F96" s="1">
+        <f t="shared" si="29"/>
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="G96" s="1">
+        <f t="shared" si="29"/>
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="H96" s="1">
+        <f t="shared" si="29"/>
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="I96" s="1">
+        <f t="shared" si="29"/>
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="J96" s="1">
+        <f t="shared" si="29"/>
+        <v>1.19716</v>
+      </c>
+      <c r="K96" s="1">
+        <f t="shared" ref="K96" si="30">K93*K95/1000</f>
+        <v>0.85263999999999995</v>
+      </c>
+    </row>
+    <row r="97" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+      <c r="K97" s="1"/>
+    </row>
+    <row r="98" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
+        <v>8</v>
+      </c>
+      <c r="E98" s="1">
+        <f t="shared" ref="E98:J98" si="31">E91-E96</f>
+        <v>0.69499999999999984</v>
+      </c>
+      <c r="F98" s="1">
+        <f t="shared" si="31"/>
+        <v>0.72500000000000009</v>
+      </c>
+      <c r="G98" s="1">
+        <f t="shared" si="31"/>
+        <v>0.79999999999999982</v>
+      </c>
+      <c r="H98" s="1">
+        <f t="shared" si="31"/>
+        <v>0.77499999999999991</v>
+      </c>
+      <c r="I98" s="1">
+        <f t="shared" si="31"/>
+        <v>0.9099999999999997</v>
+      </c>
+      <c r="J98" s="1">
+        <f t="shared" si="31"/>
+        <v>0.99283999999999994</v>
+      </c>
+      <c r="K98" s="1">
+        <f t="shared" ref="K98" si="32">K91-K96</f>
+        <v>0.69736000000000009</v>
+      </c>
+    </row>
+    <row r="99" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
+        <v>7</v>
+      </c>
+      <c r="E99" s="1">
+        <f t="shared" ref="E99:J99" si="33">E96/E91</f>
+        <v>0.63802083333333337</v>
+      </c>
+      <c r="F99" s="1">
+        <f t="shared" si="33"/>
+        <v>0.62820512820512819</v>
+      </c>
+      <c r="G99" s="1">
+        <f t="shared" si="33"/>
+        <v>0.60493827160493829</v>
+      </c>
+      <c r="H99" s="1">
+        <f t="shared" si="33"/>
+        <v>0.61250000000000004</v>
+      </c>
+      <c r="I99" s="1">
+        <f t="shared" si="33"/>
+        <v>0.57377049180327877</v>
+      </c>
+      <c r="J99" s="1">
+        <f t="shared" si="33"/>
+        <v>0.546648401826484</v>
+      </c>
+      <c r="K99" s="1">
+        <f t="shared" ref="K99" si="34">K96/K91</f>
+        <v>0.55009032258064516</v>
       </c>
     </row>
   </sheetData>

</xml_diff>